<commit_message>
Cập nhật thêm 1 kết quả khảo sát.
</commit_message>
<xml_diff>
--- a/PA5/KhaoSat/Ket qua khao sat.xlsx
+++ b/PA5/KhaoSat/Ket qua khao sat.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-9" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>STT</t>
   </si>
@@ -179,6 +179,33 @@
   </si>
   <si>
     <t>andy.need5speed@gmail.com</t>
+  </si>
+  <si>
+    <t>Huỳnh Công Toàn</t>
+  </si>
+  <si>
+    <t>Trần Huỳnh Công Toại</t>
+  </si>
+  <si>
+    <t>Lâm Quang Thiện</t>
+  </si>
+  <si>
+    <t>melodeath619@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Thuận</t>
+  </si>
+  <si>
+    <t>Trần Hưng Thuận</t>
+  </si>
+  <si>
+    <t>Võ Xuân Tiến</t>
+  </si>
+  <si>
+    <t>Giao diện nên đồng nhất hơn, nhất là về màu sắc</t>
+  </si>
+  <si>
+    <t>Một số chức năng không thực hiện được trên web tĩnh nên ko đánh giá dc</t>
   </si>
 </sst>
 </file>
@@ -189,7 +216,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -240,7 +267,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -263,6 +290,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -271,19 +335,30 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -581,654 +656,776 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.375" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="5.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75">
-      <c r="A2" s="4">
+      <c r="A2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4">
-        <v>4</v>
-      </c>
-      <c r="I2" s="4">
-        <v>2</v>
-      </c>
-      <c r="J2" s="4">
-        <v>2</v>
-      </c>
-      <c r="K2" s="4">
-        <v>2</v>
-      </c>
-      <c r="L2" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>4</v>
-      </c>
-      <c r="G3" s="4">
-        <v>4</v>
-      </c>
-      <c r="H3" s="4">
-        <v>4</v>
-      </c>
-      <c r="I3" s="4">
-        <v>4</v>
-      </c>
-      <c r="J3" s="4">
-        <v>4</v>
-      </c>
-      <c r="K3" s="4">
-        <v>4</v>
-      </c>
-      <c r="L3" s="4">
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:12" ht="15.75">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
-        <v>3</v>
-      </c>
-      <c r="H4" s="4">
-        <v>3</v>
-      </c>
-      <c r="I4" s="4">
-        <v>2</v>
-      </c>
-      <c r="J4" s="4">
-        <v>2</v>
-      </c>
-      <c r="K4" s="4">
-        <v>2</v>
-      </c>
-      <c r="L4" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="4">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="G5" s="4">
-        <v>3</v>
-      </c>
-      <c r="H5" s="4">
-        <v>4</v>
-      </c>
-      <c r="I5" s="4">
-        <v>4</v>
-      </c>
-      <c r="J5" s="4">
-        <v>4</v>
-      </c>
-      <c r="K5" s="4">
-        <v>4</v>
-      </c>
-      <c r="L5" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75">
-      <c r="A6" s="4">
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>2</v>
-      </c>
-      <c r="I6" s="4">
-        <v>2</v>
-      </c>
-      <c r="J6" s="4">
-        <v>3</v>
-      </c>
-      <c r="K6" s="4">
-        <v>4</v>
-      </c>
-      <c r="L6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75">
-      <c r="A7" s="4">
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3</v>
+      </c>
+      <c r="K7" s="2">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75">
+      <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="4">
-        <v>4</v>
-      </c>
-      <c r="E7" s="4">
-        <v>4</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
         <v>5</v>
       </c>
-      <c r="G7" s="4">
-        <v>4</v>
-      </c>
-      <c r="H7" s="4">
-        <v>4</v>
-      </c>
-      <c r="I7" s="4">
-        <v>4</v>
-      </c>
-      <c r="J7" s="4">
-        <v>4</v>
-      </c>
-      <c r="K7" s="4">
-        <v>4</v>
-      </c>
-      <c r="L7" s="4">
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2">
+        <v>4</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
+      <c r="J10" s="2">
+        <v>4</v>
+      </c>
+      <c r="K10" s="2">
+        <v>4</v>
+      </c>
+      <c r="L10" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="11" spans="1:12" ht="15.75">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="4">
-        <v>3</v>
-      </c>
-      <c r="E8" s="4">
-        <v>4</v>
-      </c>
-      <c r="F8" s="4">
-        <v>4</v>
-      </c>
-      <c r="G8" s="4">
-        <v>3</v>
-      </c>
-      <c r="H8" s="4">
-        <v>4</v>
-      </c>
-      <c r="I8" s="4">
-        <v>4</v>
-      </c>
-      <c r="J8" s="4">
-        <v>3</v>
-      </c>
-      <c r="K8" s="4">
-        <v>2</v>
-      </c>
-      <c r="L8" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="4">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4">
-        <v>2</v>
-      </c>
-      <c r="F9" s="4">
-        <v>3</v>
-      </c>
-      <c r="G9" s="4">
-        <v>2</v>
-      </c>
-      <c r="H9" s="4">
-        <v>3</v>
-      </c>
-      <c r="I9" s="4">
-        <v>3</v>
-      </c>
-      <c r="J9" s="4">
-        <v>3</v>
-      </c>
-      <c r="K9" s="4">
-        <v>2</v>
-      </c>
-      <c r="L9" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75">
-      <c r="A11" s="4">
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3</v>
+      </c>
+      <c r="I12" s="2">
+        <v>3</v>
+      </c>
+      <c r="J12" s="2">
+        <v>3</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75">
+      <c r="A13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75">
+      <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75">
-      <c r="A12" s="4">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
+      <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="4">
+      <c r="B15" s="2"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
+      <c r="A16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
+      <c r="A17" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75">
-      <c r="A14" s="4">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75">
+      <c r="A18" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75">
-      <c r="A15" s="4">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
+      <c r="A19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75">
+      <c r="A20" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="4">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75">
+      <c r="A21" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A19:L19"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
-    <hyperlink ref="C4" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C10" r:id="rId5"/>
+    <hyperlink ref="C11" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="1" max="1" width="24" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="A9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="B12" t="s">
+      <c r="B12" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="B19" t="s">
+      <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="A22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="A24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="B26" t="s">
+      <c r="B26" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="A28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="B31" t="s">
+    <row r="34" spans="1:2">
+      <c r="B34" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" s="8" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
kết quả khảo sát
</commit_message>
<xml_diff>
--- a/PA5/KhaoSat/Ket qua khao sat.xlsx
+++ b/PA5/KhaoSat/Ket qua khao sat.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -10,12 +10,12 @@
     <sheet name="1-9" sheetId="1" r:id="rId1"/>
     <sheet name="10" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>STT</t>
   </si>
@@ -206,6 +206,21 @@
   </si>
   <si>
     <t>Một số chức năng không thực hiện được trên web tĩnh nên ko đánh giá dc</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Thảo</t>
+  </si>
+  <si>
+    <t>Danh mục các món ăn nên gom nhóm lại theo dạng giống menu: món chính, món phụ, món uống…</t>
+  </si>
+  <si>
+    <t>Thiếu thông tin thời gian phục vụ của nhà hàng</t>
+  </si>
+  <si>
+    <t>Nguyễn Chí Hiếu</t>
+  </si>
+  <si>
+    <t>Trang web thiết kế khó sử dụng, cần hoàn thiện các chức năng hơn, trang web cũng không thấy có gì đặc sắc</t>
   </si>
 </sst>
 </file>
@@ -216,7 +231,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -343,6 +358,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -351,15 +375,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -660,12 +675,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.375" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
@@ -707,20 +722,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="2">
@@ -951,20 +966,20 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="2">
@@ -1081,20 +1096,20 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="7"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="2">
@@ -1117,7 +1132,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="12"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1129,20 +1144,20 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="7"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
     </row>
     <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="2">
@@ -1177,20 +1192,20 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="7"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12"/>
     </row>
     <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="2">
@@ -1249,184 +1264,205 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="9"/>
+    <col min="1" max="1" width="24" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="5" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="B39" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BMVNAH:sau khi xử xong vụ conflic
</commit_message>
<xml_diff>
--- a/PA5/KhaoSat/Ket qua khao sat.xlsx
+++ b/PA5/KhaoSat/Ket qua khao sat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="1-9" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>STT</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t xml:space="preserve"> tới vậy mình thấy không đẹp lắm. Phút thì nên để từ 0 đến 60.  Nên hiển thị tình trạng bàn hiện tại để khách hàng biết mà lựa chọn.</t>
+  </si>
+  <si>
+    <t>lightning_spkt@yahoo.com.vn</t>
+  </si>
+  <si>
+    <t>asakura255@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -385,8 +391,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -397,12 +406,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -700,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:L18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -751,20 +755,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="2">
@@ -995,20 +999,20 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="2">
@@ -1125,68 +1129,112 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>4</v>
+      </c>
+      <c r="J14" s="2">
+        <v>4</v>
+      </c>
+      <c r="K14" s="2">
+        <v>3</v>
+      </c>
+      <c r="L14" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
+      <c r="I15" s="2">
+        <v>3</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="2">
@@ -1195,7 +1243,7 @@
       <c r="B17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D17" s="2">
@@ -1233,7 +1281,7 @@
       <c r="B18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>71</v>
       </c>
       <c r="D18" s="2">
@@ -1265,20 +1313,20 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="2">
@@ -1331,9 +1379,11 @@
     <hyperlink ref="C8" r:id="rId8"/>
     <hyperlink ref="C18" r:id="rId9"/>
     <hyperlink ref="C17" r:id="rId10"/>
+    <hyperlink ref="C14" r:id="rId11"/>
+    <hyperlink ref="C15" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1341,7 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="A43" sqref="A43:N46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tổng hợp kết quả khảo sát.
</commit_message>
<xml_diff>
--- a/PA5/KhaoSat/Ket qua khao sat.xlsx
+++ b/PA5/KhaoSat/Ket qua khao sat.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1-9" sheetId="1" r:id="rId1"/>
     <sheet name="10" sheetId="2" r:id="rId2"/>
+    <sheet name="Chart" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="105">
   <si>
     <t>STT</t>
   </si>
@@ -248,17 +249,101 @@
   </si>
   <si>
     <t>asakura255@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Ánh Ngọc</t>
+  </si>
+  <si>
+    <t>anhngoc.tg@gmail.com</t>
+  </si>
+  <si>
+    <t>danh mục món nên chia nhóm</t>
+  </si>
+  <si>
+    <t>form đăng nhập thiết kế thô</t>
+  </si>
+  <si>
+    <t>nhà hàng thiếu địa chỉ, số điện thoại</t>
+  </si>
+  <si>
+    <t>Nguyễn Huỳnh Ngọc</t>
+  </si>
+  <si>
+    <t>Nên design hình ảnh lại cho đẹp</t>
+  </si>
+  <si>
+    <t>Dưới menu dọc nên có thêm 1 vài quảng cáo hay hình các món ăn. Không nên để trống</t>
+  </si>
+  <si>
+    <t>NKS001</t>
+  </si>
+  <si>
+    <t>NKS002</t>
+  </si>
+  <si>
+    <t>NKS003</t>
+  </si>
+  <si>
+    <t>NKS004</t>
+  </si>
+  <si>
+    <t>NKS005</t>
+  </si>
+  <si>
+    <t>NKS006</t>
+  </si>
+  <si>
+    <t>NKS007</t>
+  </si>
+  <si>
+    <t>NKS008</t>
+  </si>
+  <si>
+    <t>NKS009</t>
+  </si>
+  <si>
+    <t>NKS010</t>
+  </si>
+  <si>
+    <t>NKS011</t>
+  </si>
+  <si>
+    <t>NKS012</t>
+  </si>
+  <si>
+    <t>NKS013</t>
+  </si>
+  <si>
+    <t>NKS014</t>
+  </si>
+  <si>
+    <t>NKS015</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -300,6 +385,27 @@
       <family val="1"/>
       <charset val="163"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -309,7 +415,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -369,6 +475,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -377,7 +524,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -391,12 +538,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -406,7 +568,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -415,6 +576,685 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="vi-VN"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:view3D>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Câu 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart!$B$19:$F$19</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart!$B$28:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:shape val="box"/>
+        <c:axId val="68148224"/>
+        <c:axId val="90473216"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="68148224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90473216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90473216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68148224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="vi-VN"/>
+  <c:chart>
+    <c:view3D>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart!$A$20:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Câu 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Câu 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Câu 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Câu 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Câu 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Câu 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Câu 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Câu 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Câu 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart!$B$20:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart!$A$20:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Câu 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Câu 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Câu 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Câu 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Câu 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Câu 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Câu 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Câu 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Câu 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart!$C$20:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart!$A$20:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Câu 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Câu 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Câu 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Câu 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Câu 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Câu 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Câu 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Câu 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Câu 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart!$D$20:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$E$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart!$A$20:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Câu 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Câu 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Câu 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Câu 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Câu 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Câu 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Câu 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Câu 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Câu 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart!$E$20:$E$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$F$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart!$A$20:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Câu 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Câu 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Câu 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Câu 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Câu 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Câu 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Câu 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Câu 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Câu 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart!$F$20:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:shape val="box"/>
+        <c:axId val="90857472"/>
+        <c:axId val="90859008"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="90857472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90859008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90859008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90857472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -704,16 +1544,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.375" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="5.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
@@ -755,20 +1595,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="2">
@@ -999,20 +1839,20 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="2">
@@ -1129,20 +1969,20 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="2">
@@ -1189,7 +2029,7 @@
       <c r="B15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D15" s="2">
@@ -1221,20 +2061,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="13"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="24"/>
     </row>
     <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="2">
@@ -1243,7 +2083,7 @@
       <c r="B17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="15" t="s">
         <v>69</v>
       </c>
       <c r="D17" s="2">
@@ -1281,7 +2121,7 @@
       <c r="B18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="16" t="s">
         <v>71</v>
       </c>
       <c r="D18" s="2">
@@ -1313,52 +2153,94 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="13"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="24"/>
     </row>
     <row r="20" spans="1:12" ht="15.75">
-      <c r="A20" s="2">
+      <c r="A20" s="13">
         <v>14</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="B20" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="13">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13">
+        <v>3</v>
+      </c>
+      <c r="F20" s="13">
+        <v>2</v>
+      </c>
+      <c r="G20" s="13">
+        <v>2</v>
+      </c>
+      <c r="H20" s="13">
+        <v>3</v>
+      </c>
+      <c r="I20" s="13">
+        <v>3</v>
+      </c>
+      <c r="J20" s="13">
+        <v>2</v>
+      </c>
+      <c r="K20" s="13">
+        <v>2</v>
+      </c>
+      <c r="L20" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="2">
         <v>15</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2">
+        <v>2</v>
+      </c>
+      <c r="K21" s="2">
+        <v>4</v>
+      </c>
+      <c r="L21" s="2">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1381,19 +2263,18 @@
     <hyperlink ref="C17" r:id="rId10"/>
     <hyperlink ref="C14" r:id="rId11"/>
     <hyperlink ref="C15" r:id="rId12"/>
+    <hyperlink ref="C20" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:N46"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
@@ -1590,7 +2471,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15">
+    <row r="43" spans="1:14" ht="14.25">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1610,7 +2491,7 @@
       <c r="M43"/>
       <c r="N43"/>
     </row>
-    <row r="44" spans="1:14" ht="15">
+    <row r="44" spans="1:14" ht="14.25">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -1626,7 +2507,7 @@
       <c r="M44"/>
       <c r="N44"/>
     </row>
-    <row r="45" spans="1:14" ht="15">
+    <row r="45" spans="1:14" ht="14.25">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1646,7 +2527,7 @@
       <c r="M45"/>
       <c r="N45"/>
     </row>
-    <row r="46" spans="1:14" ht="15">
+    <row r="46" spans="1:14" ht="14.25">
       <c r="A46"/>
       <c r="B46" t="s">
         <v>74</v>
@@ -1664,7 +2545,809 @@
       <c r="M46"/>
       <c r="N46"/>
     </row>
+    <row r="48" spans="1:14" ht="14.25">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="B49" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="B50" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="B53" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16.5" thickBot="1">
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A3" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A4" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A5" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A6" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A7" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A8" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A9" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A10" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A11" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A12" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A14" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A15" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A16" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="20">
+        <f>COUNTIF($B$2:$B$16, "A")</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="20">
+        <f>COUNTIF($B$2:$B16, "B")</f>
+        <v>7</v>
+      </c>
+      <c r="D20" s="20">
+        <f>COUNTIF($B$2:$B16, "C")</f>
+        <v>3</v>
+      </c>
+      <c r="E20" s="20">
+        <f>COUNTIF($B$2:$B16, "D")</f>
+        <v>4</v>
+      </c>
+      <c r="F20" s="20">
+        <f>COUNTIF($B$2:$B16, "E")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75">
+      <c r="A21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="20">
+        <f>COUNTIF($C$2:$C$16, "A")</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="20">
+        <f>COUNTIF($C$2:$C17, "B")</f>
+        <v>5</v>
+      </c>
+      <c r="D21" s="20">
+        <f>COUNTIF($C$2:$C17, "C")</f>
+        <v>5</v>
+      </c>
+      <c r="E21" s="20">
+        <f>COUNTIF($C$2:$C17, "D")</f>
+        <v>5</v>
+      </c>
+      <c r="F21" s="20">
+        <f>COUNTIF($C$2:$C17, "E")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75">
+      <c r="A22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="20">
+        <f>COUNTIF($D$2:$D$16, "A")</f>
+        <v>2</v>
+      </c>
+      <c r="C22" s="20">
+        <f>COUNTIF($D$2:$D$16, "B")</f>
+        <v>4</v>
+      </c>
+      <c r="D22" s="20">
+        <f>COUNTIF($D$2:$D$16, "C")</f>
+        <v>3</v>
+      </c>
+      <c r="E22" s="20">
+        <f>COUNTIF($D$2:$D$16, "D")</f>
+        <v>4</v>
+      </c>
+      <c r="F22" s="20">
+        <f>COUNTIF($D$2:$D$16, "E")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="20">
+        <f>COUNTIF($E$2:$E$16, "A")</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="20">
+        <f>COUNTIF($E$2:$E$16, "B")</f>
+        <v>4</v>
+      </c>
+      <c r="D23" s="20">
+        <f>COUNTIF($E$2:$E$16, "C")</f>
+        <v>5</v>
+      </c>
+      <c r="E23" s="20">
+        <f>COUNTIF($E$2:$E$16, "D")</f>
+        <v>6</v>
+      </c>
+      <c r="F23" s="20">
+        <f>COUNTIF($E$2:$E$16, "E")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75">
+      <c r="A24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="20">
+        <f>COUNTIF($F$2:$F$16, "A")</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="20">
+        <f>COUNTIF($F$2:$F$16, "B")</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="20">
+        <f>COUNTIF($F$2:$F$16, "C")</f>
+        <v>6</v>
+      </c>
+      <c r="E24" s="20">
+        <f>COUNTIF($F$2:$F$16, "D")</f>
+        <v>5</v>
+      </c>
+      <c r="F24" s="20">
+        <f>COUNTIF($F$2:$F$16, "E")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75">
+      <c r="A25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="20">
+        <f>COUNTIF($G$2:$G$16, "A")</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="20">
+        <f>COUNTIF($G$2:$G$16, "B")</f>
+        <v>3</v>
+      </c>
+      <c r="D25" s="20">
+        <f>COUNTIF($G$2:$G$16, "C")</f>
+        <v>4</v>
+      </c>
+      <c r="E25" s="20">
+        <f>COUNTIF($G$2:$G$16, "D")</f>
+        <v>7</v>
+      </c>
+      <c r="F25" s="20">
+        <f>COUNTIF($G$2:$G$16, "E")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75">
+      <c r="A26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="20">
+        <f>COUNTIF($H$2:$H$16, "A")</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="20">
+        <f>COUNTIF($H$2:$H$16, "B")</f>
+        <v>6</v>
+      </c>
+      <c r="D26" s="20">
+        <f>COUNTIF($H$2:$H$16, "C")</f>
+        <v>4</v>
+      </c>
+      <c r="E26" s="20">
+        <f>COUNTIF($H$2:$H$16, "D")</f>
+        <v>5</v>
+      </c>
+      <c r="F26" s="20">
+        <f>COUNTIF($H$2:$H$16, "E")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75">
+      <c r="A27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="20">
+        <f>COUNTIF($I$2:$I$16, "A")</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="20">
+        <f>COUNTIF($I$2:$I$16, "B")</f>
+        <v>7</v>
+      </c>
+      <c r="D27" s="20">
+        <f>COUNTIF($I$2:$I$16, "C")</f>
+        <v>2</v>
+      </c>
+      <c r="E27" s="20">
+        <f>COUNTIF($I$2:$I$16, "D")</f>
+        <v>6</v>
+      </c>
+      <c r="F27" s="20">
+        <f>COUNTIF($I$2:$I$16, "E")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75">
+      <c r="A28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="20">
+        <f>COUNTIF($J$2:$J$16, "A")</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="20">
+        <f>COUNTIF($J$2:$J$16, "B")</f>
+        <v>4</v>
+      </c>
+      <c r="D28" s="20">
+        <f>COUNTIF($J$2:$J$16, "C")</f>
+        <v>5</v>
+      </c>
+      <c r="E28" s="20">
+        <f>COUNTIF($J$2:$J$16, "D")</f>
+        <v>4</v>
+      </c>
+      <c r="F28" s="20">
+        <f>COUNTIF($J$2:$J$16, "E")</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C20" formula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>